<commit_message>
Python code now gets zero crossings and calculates peak-peak without regression
</commit_message>
<xml_diff>
--- a/Calibration/Calibración Final.xlsx
+++ b/Calibration/Calibración Final.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Q\Documents\TEC\2024 - II Semestre\eWave\eWave\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C4C2AC-FC1A-4BE7-9EB5-1489725C5EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8F5405-DA64-444A-A6E4-932F0D4EEAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DD6E8BBC-5264-4291-AA6B-4364FD396A03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DD6E8BBC-5264-4291-AA6B-4364FD396A03}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration_NoBond" sheetId="5" r:id="rId1"/>
     <sheet name="Calibration_Bond" sheetId="8" r:id="rId2"/>
+    <sheet name="Wave peak-peak" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Intercepto</t>
   </si>
@@ -65,6 +66,39 @@
   <si>
     <t>D</t>
   </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Time (min)</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>Var ~0.2</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
 </sst>
 </file>
 
@@ -87,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -115,11 +149,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -143,6 +186,24 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5221,9 +5282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E54C66C-0515-4BEF-90E7-4F49CBCFD5C5}">
   <dimension ref="A2:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5469,7 +5528,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="1">
         <v>716</v>
@@ -5484,7 +5543,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="2">
         <v>736</v>
@@ -5499,7 +5558,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4"/>
@@ -5507,7 +5566,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4"/>
@@ -5515,7 +5574,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="1"/>
       <c r="C21" s="4"/>
@@ -5523,7 +5582,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="1"/>
       <c r="C22" s="4"/>
@@ -5531,122 +5590,58 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="1"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>15</v>
-      </c>
-      <c r="I23">
-        <v>30</v>
-      </c>
-      <c r="J23">
-        <v>45</v>
-      </c>
-      <c r="K23">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="F24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24">
-        <v>8.5</v>
-      </c>
-      <c r="H24">
-        <v>8.6</v>
-      </c>
-      <c r="I24">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="F25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H25">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="I25">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="F26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26">
-        <v>8.1</v>
-      </c>
-      <c r="H26">
-        <v>8.1</v>
-      </c>
-      <c r="I26">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27">
-        <v>7.4</v>
-      </c>
-      <c r="H27">
-        <v>7.5</v>
-      </c>
-      <c r="I27">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -6318,4 +6313,174 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0568ED88-4CF4-44E8-A70C-B994A9054EB5}">
+  <dimension ref="B2:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="10"/>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45</v>
+      </c>
+      <c r="G3" s="3">
+        <v>60</v>
+      </c>
+      <c r="H3" s="13">
+        <v>75</v>
+      </c>
+      <c r="I3" s="3">
+        <v>90</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E5" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="12"/>
+      <c r="F9" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrections of calibration - Now it finally works!
</commit_message>
<xml_diff>
--- a/Calibration/Calibración Final.xlsx
+++ b/Calibration/Calibración Final.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Q\Documents\TEC\2024 - II Semestre\eWave\eWave\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8F5405-DA64-444A-A6E4-932F0D4EEAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D177E11D-5637-45EC-82E4-31F13F6EC14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DD6E8BBC-5264-4291-AA6B-4364FD396A03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DD6E8BBC-5264-4291-AA6B-4364FD396A03}"/>
   </bookViews>
   <sheets>
-    <sheet name="Calibration_NoBond" sheetId="5" r:id="rId1"/>
-    <sheet name="Calibration_Bond" sheetId="8" r:id="rId2"/>
+    <sheet name="Calibration_NoBond" sheetId="8" r:id="rId1"/>
+    <sheet name="Calibration_Bond" sheetId="10" r:id="rId2"/>
     <sheet name="Wave peak-peak" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Intercepto</t>
   </si>
@@ -67,37 +67,22 @@
     <t>D</t>
   </si>
   <si>
-    <t>8.3</t>
-  </si>
-  <si>
-    <t>8.2</t>
-  </si>
-  <si>
     <t>Position</t>
   </si>
   <si>
     <t>Time (min)</t>
   </si>
   <si>
-    <t>7.2</t>
+    <t>8,6 - 8,9</t>
   </si>
   <si>
-    <t>8.7</t>
+    <t>6,9 - 7,2</t>
   </si>
   <si>
-    <t>8.6</t>
+    <t>Var ~0,2</t>
   </si>
   <si>
-    <t>8.1</t>
-  </si>
-  <si>
-    <t>7.3</t>
-  </si>
-  <si>
-    <t>Var ~0.2</t>
-  </si>
-  <si>
-    <t>8.4</t>
+    <t>Bomba ON whoops</t>
   </si>
 </sst>
 </file>
@@ -162,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -186,22 +171,25 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -348,8 +336,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.5971347331583552E-2"/>
-                  <c:y val="-0.1767202537182852"/>
+                  <c:x val="0.19698534730402795"/>
+                  <c:y val="-0.17171296296296296"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -389,52 +377,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>436</c:v>
+                  <c:v>430</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>456</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>476</c:v>
+                  <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>496</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>516</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>536</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>556</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>576</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>596</c:v>
+                  <c:v>590</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>616</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>636</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>656</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>676</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>696</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>716</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>736</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -446,52 +425,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>438.07</c:v>
+                  <c:v>429.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>458.2</c:v>
+                  <c:v>449.38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>478.75</c:v>
+                  <c:v>470.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>499.44</c:v>
+                  <c:v>490.42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>518.45000000000005</c:v>
+                  <c:v>510.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>537.24</c:v>
+                  <c:v>530.33000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>557.49</c:v>
+                  <c:v>550.27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>580.21</c:v>
+                  <c:v>569.91999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>594.79999999999995</c:v>
+                  <c:v>590.20000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>614.88</c:v>
+                  <c:v>610.37</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>635.48</c:v>
+                  <c:v>630.96</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>655.64</c:v>
+                  <c:v>651.05999999999995</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>675.97</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>696.08</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>716.58</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>745.23</c:v>
+                  <c:v>670.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -499,7 +469,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E8C1-43E3-9C85-0DB9103DCE03}"/>
+              <c16:uniqueId val="{00000001-BD12-4FBF-987D-67C3995795F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -518,8 +488,8 @@
         <c:axId val="1247600800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="756"/>
-          <c:min val="416"/>
+          <c:max val="755"/>
+          <c:min val="415"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -944,8 +914,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.10069173802769603"/>
-                  <c:y val="-0.64679024496937887"/>
+                  <c:x val="0.21902754579919934"/>
+                  <c:y val="-0.65141987459900841"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -985,52 +955,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>436</c:v>
+                  <c:v>430</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>456</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>476</c:v>
+                  <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>496</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>516</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>536</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>556</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>576</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>596</c:v>
+                  <c:v>590</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>616</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>636</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>656</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>676</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>696</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>716</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>736</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,52 +1003,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>436.2372639047469</c:v>
+                  <c:v>429.92464921969844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>456.3909296431176</c:v>
+                  <c:v>449.56987718588357</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>476.96508915248268</c:v>
+                  <c:v>470.19040015748215</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>497.67941325217913</c:v>
+                  <c:v>490.41284353503443</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>516.71176226789839</c:v>
+                  <c:v>510.31682323734964</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>535.5238526416681</c:v>
+                  <c:v>530.13123503100439</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>555.79765945746578</c:v>
+                  <c:v>549.97550279421262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>578.54437011696825</c:v>
+                  <c:v>569.53116285173724</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>593.15152278079472</c:v>
+                  <c:v>589.71379826988493</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>613.25512973690422</c:v>
+                  <c:v>609.78696179966983</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>633.87934802853056</c:v>
+                  <c:v>630.27810890320336</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>654.06304903625801</c:v>
+                  <c:v>650.28160850403003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>674.41694990367364</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>694.55059212913989</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>715.0746928562437</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>743.75837509192775</c:v>
+                  <c:v>669.88702851081052</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1095,7 +1047,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E41D-43A4-917A-A4A92E4877D9}"/>
+              <c16:uniqueId val="{00000002-72CF-4BDB-9F88-1DEE40A7DA4D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1114,8 +1066,8 @@
         <c:axId val="1247600800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="756"/>
-          <c:min val="416"/>
+          <c:max val="755"/>
+          <c:min val="415"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1526,8 +1478,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.5971347331583552E-2"/>
-                  <c:y val="-0.1767202537182852"/>
+                  <c:x val="0.19698534730402795"/>
+                  <c:y val="-0.17171296296296296"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1567,52 +1519,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>435</c:v>
+                  <c:v>430</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>455</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>495</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>515</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>535</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>555</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>575</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>595</c:v>
+                  <c:v>590</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>615</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>635</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>655</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>695</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>715</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>735</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1624,52 +1567,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>440.73</c:v>
+                  <c:v>428.74</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>460.28</c:v>
+                  <c:v>448.47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>481.4</c:v>
+                  <c:v>468.46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>505.13</c:v>
+                  <c:v>488.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>524.19000000000005</c:v>
+                  <c:v>508.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>543.1</c:v>
+                  <c:v>528.46</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>564.24</c:v>
+                  <c:v>548.67999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>584.70000000000005</c:v>
+                  <c:v>568.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>606.4</c:v>
+                  <c:v>588.09</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>626.87</c:v>
+                  <c:v>607.88</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>645.51</c:v>
+                  <c:v>627</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>665.46</c:v>
+                  <c:v>647.15</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>688.14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>705.07</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>727.55</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>746.49</c:v>
+                  <c:v>667.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1677,7 +1611,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BD12-4FBF-987D-67C3995795F2}"/>
+              <c16:uniqueId val="{00000001-F17B-4621-AF9F-9508906A9882}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2122,8 +2056,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.10069173802769603"/>
-                  <c:y val="-0.64679024496937887"/>
+                  <c:x val="0.21902754579919934"/>
+                  <c:y val="-0.65141987459900841"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2163,52 +2097,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>435</c:v>
+                  <c:v>430</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>455</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>495</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>515</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>535</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>555</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>575</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>595</c:v>
+                  <c:v>590</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>615</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>635</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>655</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>695</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>715</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>735</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2220,52 +2145,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>434.12039138548454</c:v>
+                  <c:v>429.91026186516086</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>453.27752919899996</c:v>
+                  <c:v>449.75244652458144</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>473.97311746608165</c:v>
+                  <c:v>469.85610954241298</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>497.22625712412372</c:v>
+                  <c:v>489.76869222140579</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>515.90324161136698</c:v>
+                  <c:v>510.42548253587609</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>534.43324038648609</c:v>
+                  <c:v>530.1972691757245</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>555.14842674851764</c:v>
+                  <c:v>550.53223997215036</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>575.19727788225305</c:v>
+                  <c:v>570.06266197346554</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>596.46121090288136</c:v>
+                  <c:v>590.16632499129719</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>616.51986108409176</c:v>
+                  <c:v>610.06885081035102</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>634.7852855773873</c:v>
+                  <c:v>629.29756701349959</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>654.33438528990064</c:v>
+                  <c:v>649.56213979035329</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>676.5586249630735</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>693.14841233815366</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>715.17667106182762</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>733.73606697937157</c:v>
+                  <c:v>670.39995358372357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2273,7 +2189,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-72CF-4BDB-9F88-1DEE40A7DA4D}"/>
+              <c16:uniqueId val="{00000002-C8AC-49D9-81C5-EFF8CDA2EBA2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4818,10 +4734,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="20" name="Gráfico 1">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8679F7B6-83FA-4FDC-8FBB-06496066878E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1F66D1C-297D-4AC2-A0BC-672C45FA7A07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4856,10 +4772,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Gráfico 2">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4E9C89B-0199-4D32-B362-32C652CC88AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9E27D52-8C41-4FB5-9962-1BF4E6154B9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4902,7 +4818,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1F66D1C-297D-4AC2-A0BC-672C45FA7A07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BF39F8A-DD92-4EAA-98B0-F83E2E6C0372}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4940,7 +4856,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9E27D52-8C41-4FB5-9962-1BF4E6154B9C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25BA0558-BD64-40AA-879F-EFC262BFA6F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5279,7 +5195,507 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E54C66C-0515-4BEF-90E7-4F49CBCFD5C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759A7D7B-E854-4DCE-A9EA-2115A357C041}">
+  <dimension ref="A2:K76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <f>INTERCEPT($C$3:$C$15,$B$3:$B$15)</f>
+        <v>-2.3586813186814197</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
+        <v>430</v>
+      </c>
+      <c r="C3" s="4">
+        <v>429.64</v>
+      </c>
+      <c r="D3" s="4">
+        <f>(C3-$G$2)/$G$3</f>
+        <v>429.92464921969844</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <f>SLOPE($C$3:$C$15,$B$3:$B$15)</f>
+        <v>1.0048241758241758</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <v>450</v>
+      </c>
+      <c r="C4" s="4">
+        <v>449.38</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" ref="D4:D18" si="0">(C4-$G$2)/$G$3</f>
+        <v>449.56987718588357</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>470</v>
+      </c>
+      <c r="C5" s="4">
+        <v>470.1</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>470.19040015748215</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>490</v>
+      </c>
+      <c r="C6" s="4">
+        <v>490.42</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>490.41284353503443</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>510</v>
+      </c>
+      <c r="C7" s="4">
+        <v>510.42</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>510.31682323734964</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>530</v>
+      </c>
+      <c r="C8" s="4">
+        <v>530.33000000000004</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>530.13123503100439</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>550</v>
+      </c>
+      <c r="C9" s="4">
+        <v>550.27</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>549.97550279421262</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>570</v>
+      </c>
+      <c r="C10" s="4">
+        <v>569.91999999999996</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>569.53116285173724</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>590</v>
+      </c>
+      <c r="C11" s="4">
+        <v>590.20000000000005</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>589.71379826988493</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>610</v>
+      </c>
+      <c r="C12" s="4">
+        <v>610.37</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>609.78696179966983</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>630</v>
+      </c>
+      <c r="C13" s="4">
+        <v>630.96</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>630.27810890320336</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>650</v>
+      </c>
+      <c r="C14" s="4">
+        <v>651.05999999999995</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>650.28160850403003</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="2">
+        <v>670</v>
+      </c>
+      <c r="C15" s="2">
+        <v>670.76</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>669.88702851081052</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F68" s="4"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F70" s="4"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F71" s="4"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F72" s="4"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F74" s="4"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F75" s="4"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F76" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449DDF70-ED67-4D2E-86DD-CDB8400C408B}">
   <dimension ref="A2:K76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5311,8 +5727,8 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
-        <f>INTERCEPT($C$3:$C$18,$B$3:$B$18)</f>
-        <v>2.3449941176471611</v>
+        <f>INTERCEPT($C$3:$C$15,$B$3:$B$15)</f>
+        <v>1.2603846153845097</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -5320,22 +5736,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="C3" s="4">
-        <v>438.07</v>
+        <v>428.74</v>
       </c>
       <c r="D3" s="4">
         <f>(C3-$G$2)/$G$3</f>
-        <v>436.2372639047469</v>
+        <v>429.91026186516086</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="1">
-        <f>SLOPE($C$3:$C$18,$B$3:$B$18)</f>
-        <v>0.99882573529411756</v>
+        <f>SLOPE($C$3:$C$15,$B$3:$B$15)</f>
+        <v>0.99434615384615377</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -5343,14 +5759,14 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C4" s="4">
-        <v>458.2</v>
+        <v>448.47</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" ref="D4:D18" si="0">(C4-$G$2)/$G$3</f>
-        <v>456.3909296431176</v>
+        <v>449.75244652458144</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="1"/>
@@ -5360,14 +5776,14 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="C5" s="4">
-        <v>478.75</v>
+        <v>468.46</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
-        <v>476.96508915248268</v>
+        <v>469.85610954241298</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="1"/>
@@ -5377,14 +5793,14 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="C6" s="4">
-        <v>499.44</v>
+        <v>488.26</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>497.67941325217913</v>
+        <v>489.76869222140579</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="1"/>
@@ -5394,683 +5810,146 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="C7" s="4">
-        <v>518.45000000000005</v>
+        <v>508.8</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>516.71176226789839</v>
+        <v>510.42548253587609</v>
       </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="C8" s="4">
-        <v>537.24</v>
+        <v>528.46</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>535.5238526416681</v>
+        <v>530.1972691757245</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="C9" s="4">
-        <v>557.49</v>
+        <v>548.67999999999995</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>555.79765945746578</v>
+        <v>550.53223997215036</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="C10" s="4">
-        <v>580.21</v>
+        <v>568.1</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>578.54437011696825</v>
+        <v>570.06266197346554</v>
       </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="C11" s="4">
-        <v>594.79999999999995</v>
+        <v>588.09</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>593.15152278079472</v>
+        <v>590.16632499129719</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="C12" s="4">
-        <v>614.88</v>
+        <v>607.88</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="0"/>
-        <v>613.25512973690422</v>
+        <v>610.06885081035102</v>
       </c>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="C13" s="4">
-        <v>635.48</v>
+        <v>627</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="0"/>
-        <v>633.87934802853056</v>
+        <v>629.29756701349959</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="C14" s="4">
-        <v>655.64</v>
+        <v>647.15</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="0"/>
-        <v>654.06304903625801</v>
+        <v>649.56213979035329</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
-      <c r="B15" s="1">
-        <v>676</v>
-      </c>
-      <c r="C15" s="1">
-        <v>675.97</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="B15" s="2">
+        <v>670</v>
+      </c>
+      <c r="C15" s="2">
+        <v>667.87</v>
+      </c>
+      <c r="D15" s="5">
         <f t="shared" si="0"/>
-        <v>674.41694990367364</v>
+        <v>670.39995358372357</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="1">
-        <v>696</v>
-      </c>
-      <c r="C16" s="4">
-        <v>696.08</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" si="0"/>
-        <v>694.55059212913989</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="1">
-        <v>716</v>
-      </c>
-      <c r="C17" s="4">
-        <v>716.58</v>
-      </c>
-      <c r="D17" s="4">
-        <f t="shared" si="0"/>
-        <v>715.0746928562437</v>
-      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
-      <c r="B18" s="2">
-        <v>736</v>
-      </c>
-      <c r="C18" s="5">
-        <v>745.23</v>
-      </c>
-      <c r="D18" s="5">
-        <f t="shared" si="0"/>
-        <v>743.75837509192775</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="1"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="1"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="1"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="1"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="1"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="1"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="1"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="1"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="1"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="4"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F42" s="4"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F44" s="4"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F48" s="4"/>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F49" s="4"/>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F50" s="4"/>
-    </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F52" s="4"/>
-    </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F53" s="4"/>
-    </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F54" s="4"/>
-    </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F55" s="4"/>
-    </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F56" s="4"/>
-    </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F57" s="4"/>
-    </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F58" s="4"/>
-    </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F59" s="4"/>
-    </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F60" s="4"/>
-    </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F61" s="4"/>
-    </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F62" s="4"/>
-    </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F63" s="4"/>
-    </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F64" s="4"/>
-    </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F65" s="4"/>
-    </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F66" s="4"/>
-    </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F67" s="4"/>
-    </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F68" s="4"/>
-    </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F69" s="4"/>
-    </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F70" s="4"/>
-    </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F71" s="4"/>
-    </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F72" s="4"/>
-    </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F73" s="4"/>
-    </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F74" s="4"/>
-    </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F75" s="4"/>
-    </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F76" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759A7D7B-E854-4DCE-A9EA-2115A357C041}">
-  <dimension ref="A2:K76"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <f>INTERCEPT($C$3:$C$18,$B$3:$B$18)</f>
-        <v>-2.2930514705883525</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
-        <v>435</v>
-      </c>
-      <c r="C3" s="4">
-        <v>440.73</v>
-      </c>
-      <c r="D3" s="4">
-        <f>(C3-$G$2)/$G$3</f>
-        <v>434.12039138548454</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <f>SLOPE($C$3:$C$18,$B$3:$B$18)</f>
-        <v>1.0205073529411766</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
-        <v>455</v>
-      </c>
-      <c r="C4" s="4">
-        <v>460.28</v>
-      </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D18" si="0">(C4-$G$2)/$G$3</f>
-        <v>453.27752919899996</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
-        <v>475</v>
-      </c>
-      <c r="C5" s="4">
-        <v>481.4</v>
-      </c>
-      <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>473.97311746608165</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="1">
-        <v>495</v>
-      </c>
-      <c r="C6" s="4">
-        <v>505.13</v>
-      </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>497.22625712412372</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
-        <v>515</v>
-      </c>
-      <c r="C7" s="4">
-        <v>524.19000000000005</v>
-      </c>
-      <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>515.90324161136698</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
-        <v>535</v>
-      </c>
-      <c r="C8" s="4">
-        <v>543.1</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>534.43324038648609</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
-        <v>555</v>
-      </c>
-      <c r="C9" s="4">
-        <v>564.24</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>555.14842674851764</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
-        <v>575</v>
-      </c>
-      <c r="C10" s="4">
-        <v>584.70000000000005</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>575.19727788225305</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="1">
-        <v>595</v>
-      </c>
-      <c r="C11" s="4">
-        <v>606.4</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>596.46121090288136</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="1">
-        <v>615</v>
-      </c>
-      <c r="C12" s="4">
-        <v>626.87</v>
-      </c>
-      <c r="D12" s="4">
-        <f t="shared" si="0"/>
-        <v>616.51986108409176</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
-        <v>635</v>
-      </c>
-      <c r="C13" s="4">
-        <v>645.51</v>
-      </c>
-      <c r="D13" s="4">
-        <f t="shared" si="0"/>
-        <v>634.7852855773873</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
-        <v>655</v>
-      </c>
-      <c r="C14" s="4">
-        <v>665.46</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" si="0"/>
-        <v>654.33438528990064</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="1">
-        <v>675</v>
-      </c>
-      <c r="C15" s="1">
-        <v>688.14</v>
-      </c>
-      <c r="D15" s="4">
-        <f t="shared" si="0"/>
-        <v>676.5586249630735</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1">
-        <v>695</v>
-      </c>
-      <c r="C16" s="4">
-        <v>705.07</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" si="0"/>
-        <v>693.14841233815366</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="1">
-        <v>715</v>
-      </c>
-      <c r="C17" s="4">
-        <v>727.55</v>
-      </c>
-      <c r="D17" s="4">
-        <f t="shared" si="0"/>
-        <v>715.17667106182762</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="2">
-        <v>735</v>
-      </c>
-      <c r="C18" s="5">
-        <v>746.49</v>
-      </c>
-      <c r="D18" s="5">
-        <f t="shared" si="0"/>
-        <v>733.73606697937157</v>
-      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
@@ -6317,10 +6196,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0568ED88-4CF4-44E8-A70C-B994A9054EB5}">
-  <dimension ref="B2:J9"/>
+  <dimension ref="B2:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6328,23 +6207,23 @@
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="10"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="11"/>
       <c r="C3" s="3">
         <v>0</v>
       </c>
@@ -6360,15 +6239,17 @@
       <c r="G3" s="3">
         <v>60</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="3">
         <v>75</v>
       </c>
       <c r="I3" s="3">
         <v>90</v>
       </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J3" s="3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -6382,20 +6263,23 @@
         <v>8.6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H4" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K4" s="14"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -6408,19 +6292,24 @@
       <c r="E5" s="1">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F5" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G5" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H5" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -6433,19 +6322,24 @@
       <c r="E6" s="1">
         <v>8.1</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F6" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G6" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -6458,22 +6352,29 @@
       <c r="E7" s="2">
         <v>7.6</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>7.3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
+      <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
-      <c r="F9" s="11" t="s">
-        <v>18</v>
+      <c r="I9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First version of python integrated code to measure amplitue
</commit_message>
<xml_diff>
--- a/Calibration/Calibración Final.xlsx
+++ b/Calibration/Calibración Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Q\Documents\TEC\2024 - II Semestre\eWave\eWave\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D177E11D-5637-45EC-82E4-31F13F6EC14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308F76C8-7C77-4AC5-9A75-7EEAFF26BAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DD6E8BBC-5264-4291-AA6B-4364FD396A03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DD6E8BBC-5264-4291-AA6B-4364FD396A03}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration_NoBond" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Intercepto</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Position</t>
   </si>
   <si>
-    <t>Time (min)</t>
-  </si>
-  <si>
     <t>8,6 - 8,9</t>
   </si>
   <si>
@@ -82,7 +79,13 @@
     <t>Var ~0,2</t>
   </si>
   <si>
-    <t>Bomba ON whoops</t>
+    <t>Measurement (very far apart)</t>
+  </si>
+  <si>
+    <t>Bomba ON</t>
+  </si>
+  <si>
+    <t>Whoops</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,15 +182,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5198,7 +5192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759A7D7B-E854-4DCE-A9EA-2115A357C041}">
   <dimension ref="A2:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5265,7 +5259,7 @@
         <v>449.38</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D18" si="0">(C4-$G$2)/$G$3</f>
+        <f t="shared" ref="D4:D15" si="0">(C4-$G$2)/$G$3</f>
         <v>449.56987718588357</v>
       </c>
       <c r="E4" s="4"/>
@@ -5447,9 +5441,9 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
@@ -5765,7 +5759,7 @@
         <v>448.47</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D18" si="0">(C4-$G$2)/$G$3</f>
+        <f t="shared" ref="D4:D15" si="0">(C4-$G$2)/$G$3</f>
         <v>449.75244652458144</v>
       </c>
       <c r="E4" s="4"/>
@@ -5947,9 +5941,9 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
@@ -6196,11 +6190,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0568ED88-4CF4-44E8-A70C-B994A9054EB5}">
-  <dimension ref="B2:K9"/>
+  <dimension ref="B2:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6211,42 +6203,46 @@
       <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="C2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="G3" s="3">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="H3" s="3">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="I3" s="3">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="J3" s="3">
-        <v>105</v>
+        <v>8</v>
+      </c>
+      <c r="K3" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
@@ -6263,7 +6259,7 @@
         <v>8.6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1">
         <v>8.6999999999999993</v>
@@ -6277,7 +6273,9 @@
       <c r="J4" s="1">
         <v>8.1999999999999993</v>
       </c>
-      <c r="K4" s="14"/>
+      <c r="K4" s="1">
+        <v>8.4</v>
+      </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
@@ -6302,12 +6300,14 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" s="1">
         <v>8.4</v>
       </c>
-      <c r="K5" s="14"/>
+      <c r="K5" s="1">
+        <v>8.3000000000000007</v>
+      </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
@@ -6337,7 +6337,9 @@
       <c r="J6" s="1">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K6" s="14"/>
+      <c r="K6" s="1">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
@@ -6367,20 +6369,28 @@
       <c r="J7" s="2">
         <v>7.5</v>
       </c>
+      <c r="K7" s="2">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="F9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I10" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>